<commit_message>
update questions scale wvs
</commit_message>
<xml_diff>
--- a/data/demo_data/wvs/questions.xlsx
+++ b/data/demo_data/wvs/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaca253\Documents\datomatisation\datomatisation-dev\data\demo_data\wvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED719E9E-A6E8-4AC9-9528-43D1F51FB3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B63748-3741-4018-8469-0EC7F835AC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35715" yWindow="855" windowWidth="27240" windowHeight="19065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32865" yWindow="1275" windowWidth="22605" windowHeight="19065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Key</t>
   </si>
@@ -36,15 +36,9 @@
     <t>Q164</t>
   </si>
   <si>
-    <t>How important is God in your life? (on a scale 1 = not at all important; 2 = not at all important; 3 = unimportant; 4 = somewhat unimportant; 5 = neither important nor unimportant; 6 = neither important nor unimportant; 7 = somewhat important; 8 = important; 9 = very important; 10 = very important)</t>
-  </si>
-  <si>
     <t>Q8</t>
   </si>
   <si>
-    <t>Here is a list of qualities that children can be encouraged to learn at home. Which, if any, do you consider to be especially important? (on a scale 1 = mentioned; 2 = did not mention)</t>
-  </si>
-  <si>
     <t>Q14</t>
   </si>
   <si>
@@ -57,135 +51,69 @@
     <t>Q184</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Abortion (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q254</t>
   </si>
   <si>
-    <t>How proud are you to be of the nationality of this country? (on a scale 1 = yery proud; 2 = quite proud; 3 = not very proud; 4 = not at all proud; 5 = I am not [country's nationality])</t>
-  </si>
-  <si>
     <t>Q45</t>
   </si>
   <si>
-    <t>In the future, would it be a good thing if we had greater respect for authority? (on a scale 1 = good; 2 = neither good nor bad; 3 = bad)</t>
-  </si>
-  <si>
     <t>Q3</t>
   </si>
   <si>
-    <t>How important is leisure time to you? (on a scale 1 = very important; 2 = rather important; 3 = not very important; 4 = not at all important)</t>
-  </si>
-  <si>
     <t>Q5</t>
   </si>
   <si>
-    <t>How important is work to you? (on a scale 1 = very important; 2 = rather important; 3 = not very important; 4 = not at all important)</t>
-  </si>
-  <si>
     <t>Q40</t>
   </si>
   <si>
-    <t>Do you think that work is a duty towards society? (on a scale 1 = agree strongly; 2 = agree; 3 = neither agree nor disagree; 4 = disagree; 5 = disagree strongly)</t>
-  </si>
-  <si>
     <t>Q41</t>
   </si>
   <si>
-    <t>Do you think work should always come first, even if it means no spare time? (on a scale 1 = agree strongly; 2 = agree; 3 = neither agree nor disagree; 4 = disagree; 5 = disagree strongly)</t>
-  </si>
-  <si>
     <t>Q43</t>
   </si>
   <si>
-    <t>In the future, would it be a good thing if less importance is placed on work (on a scale 1 = good; 2 = neither good nor bad; 3 = bad)</t>
-  </si>
-  <si>
     <t>Q131</t>
   </si>
   <si>
-    <t>Could you tell me how secure do you feel these days in your neighborhood? (on a scale 1 = very secure; 2 = quite secure; 3 = not very secure; 4 = not at all secure)</t>
-  </si>
-  <si>
     <t>Q142</t>
   </si>
   <si>
-    <t>To what degree are you worried about the following situations? Losing my job or not finding a job (on a scale 1 = very much; 2 = a good deal; 3 = not much; 4 = not at all)</t>
-  </si>
-  <si>
     <t>Q150</t>
   </si>
   <si>
-    <t>Most people consider both freedom and security to be important, but if you had to choose between them, do you think security is more important than freedom (on a scale 1 = freedom; 2 = security)</t>
-  </si>
-  <si>
     <t>Q46</t>
   </si>
   <si>
-    <t>Do you feel happy? (on a scale 1 = very happy; 2 = rather happy; 3 = not very happy; 4 = not at all happy)</t>
-  </si>
-  <si>
     <t>Q49</t>
   </si>
   <si>
-    <t>How satisfied are you with your life? (on a scale 1 = completely dissatisfied; 2 = almost completely dissatisfied; 3 = dissatisfied; 4 = somewhat dissatisfied; 5 = neither important nor dissatisfied; 6 = neither important nor dissatisfied; 7 = somewhat satisfied; 8 = satisfied; 9 = almost completely satisfied; 10 = completely satisfied)</t>
-  </si>
-  <si>
     <t>Q22</t>
   </si>
   <si>
-    <t>On this list are various groups of people. Could you please mention any that you would not like to have as neighbors? (on a scale 1 = mentioned; 2 = did not mention)</t>
-  </si>
-  <si>
     <t>Q182</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Homosexuality (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q209</t>
   </si>
   <si>
-    <t>I’m going to read out some forms of political action that people can take, and I'd like you to tell me, for each one, whether you have done any of these things, whether you might do it or would never under any circumstances do it: signing a petition (on a scale 1 = have done; 2 = might do; 3 = would never do)</t>
-  </si>
-  <si>
     <t>Q218</t>
   </si>
   <si>
-    <t>I’m going to read out some other forms of political action that people can take using Internet and social media tools like Facebook, Twitter etc., and I'd like you to tell me, for each one, whether you have done any of these things, whether you might do it or would never under any circumstances do it: signing an electronic petition (on a scale 1 = have done; 2 = might do; 3 = would never do)</t>
-  </si>
-  <si>
     <t>Q57</t>
   </si>
   <si>
-    <t>Most people can be trusted (on a scale 1 = most people can be trusted; 2 = one needs to be very careful)</t>
-  </si>
-  <si>
     <t>Q58</t>
   </si>
   <si>
-    <t>How much do you trust your family? (on a scale 1 = trust completely; 2 = trust somewhat; 3 = do not trust very much; 4 = do not trust at all)</t>
-  </si>
-  <si>
     <t>Q59</t>
   </si>
   <si>
-    <t>How much do you trust your neighborhood? (on a scale 1 = trust completely; 2 = trust somewhat; 3 = do not trust very much; 4 = do not trust at all)</t>
-  </si>
-  <si>
     <t>Q60</t>
   </si>
   <si>
-    <t>How much do you trust people you know personally? (on a scale 1 = trust completely; 2 = trust somewhat; 3 = do not trust very much; 4 = do not trust at all)</t>
-  </si>
-  <si>
     <t>Q61</t>
   </si>
   <si>
-    <t>How much do you trust people you meet for the first time? (on a scale 1 = trust completely; 2 = trust somewhat; 3 = do not trust very much; 4 = do not trust at all)</t>
-  </si>
-  <si>
     <t>Q62</t>
   </si>
   <si>
@@ -195,115 +123,196 @@
     <t>Q63</t>
   </si>
   <si>
-    <t>How much do you trust people of another nationality? (on a scale 1 = trust completely; 2 = trust somewhat; 3 = do not trust very much; 4 = do not trust at all)</t>
-  </si>
-  <si>
     <t>Q102</t>
   </si>
   <si>
-    <t>Are you a member of a consumer organization? (on a scale 2 = are an active member; 1 = are an inactive member; 0 = don't belong)</t>
-  </si>
-  <si>
     <t>Q101</t>
   </si>
   <si>
-    <t>Are you a member of a charitable or humanitarian organization? (on a scale 2 = are an active member; 1 = are an inactive member; 0 = don't belong)</t>
-  </si>
-  <si>
     <t>Q100</t>
   </si>
   <si>
-    <t>Are you a member of a professional organization? (on a scale 2 = are an active member; 1 = are an inactive member; 0 = don't belong)</t>
-  </si>
-  <si>
     <t>Q103</t>
   </si>
   <si>
-    <t>Are you a member of a self-help or mutual aid group? (on a scale 2 = are an active member; 1 = are an inactive member; 0 = don't belong)</t>
-  </si>
-  <si>
     <t>Q179</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Stealing property (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q181</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Someone accepting a bribe in the course of their duties (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q180</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Cheating on taxes if you have a chance (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q191</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Violence against other people (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q189</t>
   </si>
   <si>
-    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: For a man to beat his wife (on a scale 1 = never justifiable; 2 = almost never justifiable; 3 = unjustifiable; 4 = sometimes unjustifiable; 5 = neither justifiable nor unjustifiable; 6 = neither justifiable nor unjustifiable; 7 = sometimes justifiable; 8 = justifiable; 9 = almost always justifiable; 10 = always justifiable)</t>
-  </si>
-  <si>
     <t>Q73</t>
   </si>
   <si>
-    <t>How much confidence do you have in the parliament? (on a scale 1 = a great deal; 2 = quite a lot; 3 = not very much; 4 = none at all)</t>
-  </si>
-  <si>
     <t>Q71</t>
   </si>
   <si>
-    <t>How much confidence do you have in the government? (on a scale 1 = a great deal; 2 = quite a lot; 3 = not very much; 4 = none at all)</t>
-  </si>
-  <si>
     <t>Q74</t>
   </si>
   <si>
-    <t>How much confidence do you have in the civil services (on a scale 1 = a great deal; 2 = quite a lot; 3 = not very much; 4 = none at all)</t>
-  </si>
-  <si>
     <t>Q72</t>
   </si>
   <si>
-    <t>How much confidence do you have in political parties? (on a scale 1 = a great deal; 2 = quite a lot; 3 = not very much; 4 = none at all)</t>
-  </si>
-  <si>
     <t>Q70</t>
   </si>
   <si>
-    <t>How much confidence do you have in the justice system/courts? (on a scale 1 = a great deal; 2 = quite a lot; 3 = not very much; 4 = none at all)</t>
-  </si>
-  <si>
     <t>Q148</t>
   </si>
   <si>
-    <t>To what degree are you worried about the following situations? A civil war (on a scale 1 = very much; 2 = a good deal; 3 = not much; 4 = not at all)</t>
-  </si>
-  <si>
     <t>Q147</t>
   </si>
   <si>
-    <t>To what degree are you worried about the following situations? A terrorist attack (on a scale 1 = very much; 2 = a good deal; 3 = not much; 4 = not at all)</t>
-  </si>
-  <si>
     <t>Q146</t>
   </si>
   <si>
-    <t>To what degree are you worried about the following situations? A war involving my country (on a scale 1 = very much; 2 = a good deal; 3 = not much; 4 = not at all)</t>
-  </si>
-  <si>
     <t>Q143</t>
   </si>
   <si>
-    <t>To what degree are you worried about the following situations? Not being able to give one's children a good education (on a scale 1 = very much; 2 = a good deal; 3 = not much; 4 = not at all)</t>
+    <t>How important is God in your life? (on a scale of ' not at all important' to 'very important')</t>
+  </si>
+  <si>
+    <t>Here is a list of qualities that children can be encouraged to learn at home. Which, if any, do you consider to be especially important? Independence (on a scale of 'mentioned' to 'did not mention')</t>
+  </si>
+  <si>
+    <t>Here is a list of qualities that children can be encouraged to learn at home. Which, if any, do you consider to be especially important? Determination, perseverance (on a scale of 'mentioned' to 'did not mention')</t>
+  </si>
+  <si>
+    <t>Here is a list of qualities that children can be encouraged to learn at home. Which, if any, do you consider to be especially important? Religious faith (on a scale of 'mentioned' to 'did not mention')</t>
+  </si>
+  <si>
+    <t>Here is a list of qualities that children can be encouraged to learn at home. Which, if any, do you consider to be especially important? Obedience (on a scale of 'mentioned' to 'did not mention')</t>
+  </si>
+  <si>
+    <t>In the future, would it be a good thing if we had greater respect for authority? (on a scale of 'good' to 'bad')</t>
+  </si>
+  <si>
+    <t>How important is leisure time to you? (on a scale of 'very important' to 'not at all important')</t>
+  </si>
+  <si>
+    <t>How proud are you to be of the nationality of this country? (on a scale fo 'very proud' to  'I am not from this country')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Abortion (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>How important is work to you? (on a scale of 'very important' to 'not at all important')</t>
+  </si>
+  <si>
+    <t>Do you think that work is a duty towards society? (on a scale of 'agree strongly' to 'disagree strongly')</t>
+  </si>
+  <si>
+    <t>Do you think work should always come first, even if it means no spare time? (on a scale of 'agree strongly' to 'disagree strongly')</t>
+  </si>
+  <si>
+    <t>In the future, would it be a good thing if less importance is placed on work?  (on a scale of 'good' to 'bad')</t>
+  </si>
+  <si>
+    <t>Could you tell me how secure do you feel these days in your neighborhood? (on a scale of 'very secure' to 'not at all secure')</t>
+  </si>
+  <si>
+    <t>To what degree are you worried about the following situations? Losing my job or not finding a job (on a scaleof 'very much' to 'not at all')</t>
+  </si>
+  <si>
+    <t>Most people consider both freedom and security to be important, but if you had to choose between them, do you think security is more important than freedom (on a scale of 'freedom' to 'security')</t>
+  </si>
+  <si>
+    <t>Do you feel happy? (on a scale of 'very happy' to 'not at all happy')</t>
+  </si>
+  <si>
+    <t>How satisfied are you with your life? (on a scale of 'completely dissatisfied' to 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>On this list are various groups of people. Could you please mention any that you would not like to have as neighbors? (on a scale of 'mentioned' to 'did not mention')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Homosexuality (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>I’m going to read out some forms of political action that people can take, and I'd like you to tell me, for each one, whether you have done any of these things, whether you might do it or would never under any circumstances do it: signing a petition (on a scale of 'have done' to 'would never do')</t>
+  </si>
+  <si>
+    <t>I’m going to read out some other forms of political action that people can take using Internet and social media tools like Facebook, Twitter etc., and I'd like you to tell me, for each one, whether you have done any of these things, whether you might do it or would never under any circumstances do it: signing an electronic petition (on a scale of 'have done' to 'would never do')</t>
+  </si>
+  <si>
+    <t>Most people can be trusted (on a scale of 'most people can be trusted' to  'one needs to be very careful')</t>
+  </si>
+  <si>
+    <t>How much do you trust your family? (on a scale of 'trust completely' to 'do not trust at all')</t>
+  </si>
+  <si>
+    <t>How much do you trust your neighborhood? (on a scale of 'trust completely to 'do not trust at all')</t>
+  </si>
+  <si>
+    <t>How much do you trust people you know personally? (on a scale of 'trust completely to 'do not trust at all')</t>
+  </si>
+  <si>
+    <t>How much do you trust people you meet for the first time? (on a scale of 'trust completely to 'do not trust at all')</t>
+  </si>
+  <si>
+    <t>How much do you trust people of another nationality? (on a scale of 'trust completely to 'do not trust at all')</t>
+  </si>
+  <si>
+    <t>Are you a member of a consumer organization? (on a scale of 'are an active member' to 'don't belong')</t>
+  </si>
+  <si>
+    <t>Are you a member of a charitable or humanitarian organization?  (on a scale of 'are an active member' to 'don't belong')</t>
+  </si>
+  <si>
+    <t>Are you a member of a professional organization?  (on a scale of 'are an active member' to 'don't belong')</t>
+  </si>
+  <si>
+    <t>Are you a member of a self-help or mutual aid group?  (on a scale of 'are an active member' to 'don't belong')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Stealing property (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Someone accepting a bribe in the course of their duties (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Cheating on taxes if you have a chance (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: Violence against other people (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>Please tell me for each of the following actions whether you think it can always be justified, never be justified, or something in between: For a man to beat his wife (on a scale of 'never justifiable' to 'always justifiable')</t>
+  </si>
+  <si>
+    <t>How much confidence do you have in the parliament? (on a scale of ' a great deal' to 'none at all')</t>
+  </si>
+  <si>
+    <t>How much confidence do you have in the government? (on a scale of ' a great deal' to 'none at all')</t>
+  </si>
+  <si>
+    <t>How much confidence do you have in the civil services (on a scale of ' a great deal' to 'none at all')</t>
+  </si>
+  <si>
+    <t>How much confidence do you have in political parties? (on a scale of ' a great deal' to 'none at all')</t>
+  </si>
+  <si>
+    <t>How much confidence do you have in the justice system/courts? (on a scale of ' a great deal' to 'none at all')</t>
+  </si>
+  <si>
+    <t>To what degree are you worried about the following situations? A civil war (on a scale of 'very much' to ' not at all')</t>
+  </si>
+  <si>
+    <t>To what degree are you worried about the following situations? A terrorist attack (on a scale of 'very much' to ' not at all')</t>
+  </si>
+  <si>
+    <t>To what degree are you worried about the following situations? A war involving my country (on a scale of 'very much' to ' not at all')</t>
+  </si>
+  <si>
+    <t>To what degree are you worried about the following situations? Not being able to give one's children a good education (on a scale of 'very much' to ' not at all')</t>
   </si>
 </sst>
 </file>
@@ -359,10 +368,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,11 +683,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -687,376 +704,376 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
+      <c r="B7" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" t="s">
-        <v>52</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" t="s">
-        <v>54</v>
+        <v>29</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" t="s">
-        <v>56</v>
+        <v>31</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
+        <v>32</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s">
-        <v>60</v>
+        <v>33</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" t="s">
-        <v>62</v>
+        <v>34</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" t="s">
-        <v>76</v>
+        <v>41</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
+        <v>42</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" t="s">
-        <v>80</v>
+        <v>43</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" t="s">
-        <v>84</v>
+        <v>45</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" t="s">
-        <v>92</v>
+        <v>49</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>